<commit_message>
feet(ttest_ind) : calculate ttest_ind
</commit_message>
<xml_diff>
--- a/Sensa.xlsx
+++ b/Sensa.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamad\Desktop\TempPractice\SensaPValue\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0D056A7-97AA-4B37-BFB8-873EF7AE76F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD989F8C-19EC-4E19-931B-56C7BA5CCE4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$80</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Sheet1!$A$1:$C$80</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -41,9 +38,39 @@
     <t>Project Name</t>
   </si>
   <si>
+    <t>Size(kb)</t>
+  </si>
+  <si>
     <t>Number of test</t>
   </si>
   <si>
+    <t>our(per)</t>
+  </si>
+  <si>
+    <t>our(rec)</t>
+  </si>
+  <si>
+    <t>our(f1)</t>
+  </si>
+  <si>
+    <t>cod2vec(per)</t>
+  </si>
+  <si>
+    <t>cod2vec(rec)</t>
+  </si>
+  <si>
+    <t>cod2vec(f1)</t>
+  </si>
+  <si>
+    <t>cod2seq(per)</t>
+  </si>
+  <si>
+    <t>cod2seq(rec)</t>
+  </si>
+  <si>
+    <t>cod2seq(f1)</t>
+  </si>
+  <si>
     <t>Activiti__Activiti</t>
   </si>
   <si>
@@ -279,49 +306,25 @@
   </si>
   <si>
     <t>zzz40500__android-shapeLoadingView</t>
-  </si>
-  <si>
-    <t>Size(kb)</t>
-  </si>
-  <si>
-    <t>our(per)</t>
-  </si>
-  <si>
-    <t>our(rec)</t>
-  </si>
-  <si>
-    <t>our(f1)</t>
-  </si>
-  <si>
-    <t>cod2vec(per)</t>
-  </si>
-  <si>
-    <t>cod2vec(rec)</t>
-  </si>
-  <si>
-    <t>cod2vec(f1)</t>
-  </si>
-  <si>
-    <t>cod2seq(per)</t>
-  </si>
-  <si>
-    <t>cod2seq(rec)</t>
-  </si>
-  <si>
-    <t>cod2seq(f1)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -332,7 +335,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -344,23 +354,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -407,20 +426,20 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -450,12 +469,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -494,204 +513,231 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:tint val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:L80"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.25" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="11.625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>81</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>85</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>88</v>
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="2">
         <v>12300</v>
@@ -699,40 +745,40 @@
       <c r="C2" s="2">
         <v>22</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="3">
         <v>76.89</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="3">
         <v>71.66</v>
       </c>
       <c r="F2" s="3">
-        <f>2*(D2*E2)/(D2+E2)</f>
+        <f t="shared" ref="F2:F31" si="0">2*(D2*E2)/(D2+E2)</f>
         <v>74.18293369235947</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="3">
         <v>53.18</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="3">
         <v>32.5</v>
       </c>
-      <c r="I2" s="2">
-        <f>2*(G2*H2)/(G2+H2)</f>
+      <c r="I2" s="3">
+        <f t="shared" ref="I2:I13" si="1">2*(G2*H2)/(G2+H2)</f>
         <v>40.344304388422032</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="3">
         <v>64.31</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="3">
         <v>53.63</v>
       </c>
-      <c r="L2" s="2">
-        <f>2*(J2*K2)/(J2+K2)</f>
+      <c r="L2" s="3">
+        <f t="shared" ref="L2:L13" si="2">2*(J2*K2)/(J2+K2)</f>
         <v>58.486438867220627</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
+    <row r="3" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B3" s="2">
         <v>640</v>
@@ -743,21 +789,21 @@
       <c r="D3" s="2">
         <v>75</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>60.66</v>
       </c>
       <c r="F3" s="3">
-        <f t="shared" ref="F3:F52" si="0">2*(D3*E3)/(D3+E3)</f>
+        <f t="shared" si="0"/>
         <v>67.072091994692613</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="2">
         <v>50</v>
       </c>
       <c r="H3" s="2">
         <v>50</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I52" si="1">2*(G3*H3)/(G3+H3)</f>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="J3" s="2">
@@ -767,13 +813,13 @@
         <v>50</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" ref="L3:L52" si="2">2*(J3*K3)/(J3+K3)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B4" s="2">
         <v>584</v>
@@ -784,37 +830,37 @@
       <c r="D4" s="2">
         <v>50</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>58.33</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" si="0"/>
         <v>53.844733684113358</v>
       </c>
-      <c r="G4" s="1">
-        <v>50</v>
-      </c>
-      <c r="H4" s="2">
+      <c r="G4" s="2">
+        <v>50</v>
+      </c>
+      <c r="H4" s="3">
         <v>58.33</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="3">
         <f t="shared" si="1"/>
         <v>53.844733684113358</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="3">
         <v>45.22</v>
       </c>
-      <c r="K4" s="2">
+      <c r="K4" s="3">
         <v>40.659999999999997</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="3">
         <f t="shared" si="2"/>
         <v>42.818938053097341</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>5</v>
+    <row r="5" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B5" s="2">
         <v>12</v>
@@ -825,14 +871,14 @@
       <c r="D5" s="2">
         <v>50</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="2">
         <v>50</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G5" s="1">
+      <c r="G5" s="2">
         <v>50</v>
       </c>
       <c r="H5" s="2">
@@ -853,9 +899,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
+    <row r="6" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B6" s="2">
         <v>192</v>
@@ -866,14 +912,14 @@
       <c r="D6" s="2">
         <v>100</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="2">
         <v>100</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="2">
         <v>50</v>
       </c>
       <c r="H6" s="2">
@@ -894,9 +940,9 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>7</v>
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B7" s="2">
         <v>22700</v>
@@ -904,40 +950,40 @@
       <c r="C7" s="2">
         <v>50</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>49.16</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <v>48.5</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>48.827769813639151</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="3">
         <v>54.83</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="3">
         <v>49.66</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="3">
         <f t="shared" si="1"/>
         <v>52.117098286917404</v>
       </c>
       <c r="J7" s="2">
         <v>50</v>
       </c>
-      <c r="K7" s="2">
+      <c r="K7" s="3">
         <v>44.66</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="3">
         <f t="shared" si="2"/>
         <v>47.179378829495036</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
+    <row r="8" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B8" s="2">
         <v>40200</v>
@@ -945,40 +991,40 @@
       <c r="C8" s="2">
         <v>101</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>64.78</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="3">
         <v>61.63</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>63.165752709437555</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="3">
         <v>58.99</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="3">
         <v>52.22</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="3">
         <f t="shared" si="1"/>
         <v>55.398935347540686</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="3">
         <v>57.17</v>
       </c>
-      <c r="K8" s="2">
+      <c r="K8" s="3">
         <v>52.47</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="3">
         <f t="shared" si="2"/>
         <v>54.719261218533376</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
+    <row r="9" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B9" s="2">
         <v>8460</v>
@@ -986,40 +1032,40 @@
       <c r="C9" s="2">
         <v>21</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>73.41</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="3">
         <v>72.22</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>72.81013802101215</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="3">
         <v>69.84</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="3">
         <v>53.09</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="3">
         <f t="shared" si="1"/>
         <v>60.323852599040109</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="3">
         <v>70.63</v>
       </c>
-      <c r="K9" s="2">
+      <c r="K9" s="3">
         <v>65.87</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="3">
         <f t="shared" si="2"/>
         <v>68.167005128205133</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
+    <row r="10" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B10" s="2">
         <v>10100</v>
@@ -1030,37 +1076,37 @@
       <c r="D10" s="2">
         <v>74</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="3">
         <v>69.66</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" si="0"/>
         <v>71.764443825699573</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="3">
         <v>35.33</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="3">
         <v>33.46</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="3">
         <f t="shared" si="1"/>
         <v>34.369582788195956</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="3">
         <v>38.659999999999997</v>
       </c>
-      <c r="K10" s="2">
+      <c r="K10" s="3">
         <v>47.46</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="3">
         <f t="shared" si="2"/>
         <v>42.610394797956339</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
+    <row r="11" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B11" s="2">
         <v>168</v>
@@ -1071,14 +1117,14 @@
       <c r="D11" s="2">
         <v>75</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="2">
         <v>75</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="2">
         <v>75</v>
       </c>
       <c r="H11" s="2">
@@ -1099,9 +1145,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>12</v>
+    <row r="12" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B12" s="2">
         <v>1780</v>
@@ -1109,40 +1155,40 @@
       <c r="C12" s="2">
         <v>4</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>55.2</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="3">
         <v>51.33</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" si="0"/>
         <v>53.194705716699524</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="3">
         <v>50.25</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="3">
         <v>42.85</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="3">
         <f t="shared" si="1"/>
         <v>46.255907626208383</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="3">
         <v>51.25</v>
       </c>
-      <c r="K12" s="2">
+      <c r="K12" s="3">
         <v>44.5</v>
       </c>
-      <c r="L12" s="2">
+      <c r="L12" s="3">
         <f t="shared" si="2"/>
         <v>47.637075718015666</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>13</v>
+    <row r="13" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B13" s="2">
         <v>256</v>
@@ -1153,37 +1199,37 @@
       <c r="D13" s="2">
         <v>75</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="3">
         <v>54.5</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" si="0"/>
         <v>63.127413127413128</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="3">
         <v>62.36</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="3">
         <v>40.33</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="3">
         <f t="shared" si="1"/>
         <v>48.981961242574741</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="3">
         <v>66.33</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="3">
         <v>62.5</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="3">
         <f t="shared" si="2"/>
         <v>64.358068772801374</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
-        <v>14</v>
+    <row r="14" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B14" s="2">
         <v>152</v>
@@ -1194,14 +1240,14 @@
       <c r="D14" s="2">
         <v>50</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="2">
         <v>50</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="2">
         <v>0</v>
       </c>
       <c r="H14" s="2">
@@ -1213,16 +1259,16 @@
       <c r="J14" s="2">
         <v>0</v>
       </c>
-      <c r="K14" s="1">
+      <c r="K14" s="2">
         <v>0</v>
       </c>
       <c r="L14" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
-        <v>15</v>
+    <row r="15" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B15" s="2">
         <v>144</v>
@@ -1233,14 +1279,14 @@
       <c r="D15" s="2">
         <v>50</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="2">
         <v>50</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="2">
         <v>0</v>
       </c>
       <c r="H15" s="2">
@@ -1259,9 +1305,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
-        <v>16</v>
+    <row r="16" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B16" s="2">
         <v>3250</v>
@@ -1269,40 +1315,40 @@
       <c r="C16" s="2">
         <v>8</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>59.89</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>54.66</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" si="0"/>
         <v>57.155607158446095</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="3">
         <v>46.18</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="3">
         <v>45.5</v>
       </c>
-      <c r="I16" s="2">
-        <f t="shared" si="1"/>
+      <c r="I16" s="3">
+        <f t="shared" ref="I16:I31" si="3">2*(G16*H16)/(G16+H16)</f>
         <v>45.837478184991269</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="3">
         <v>57.31</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="3">
         <v>53.63</v>
       </c>
-      <c r="L16" s="2">
-        <f>2*(J16*K16)/(J16+K16)</f>
+      <c r="L16" s="3">
+        <f t="shared" ref="L16:L31" si="4">2*(J16*K16)/(J16+K16)</f>
         <v>55.408965206417896</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
-        <v>17</v>
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B17" s="2">
         <v>124</v>
@@ -1313,37 +1359,37 @@
       <c r="D17" s="2">
         <v>100</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="2">
         <v>100</v>
       </c>
       <c r="F17" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="3">
         <v>33.33</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="3">
         <v>33.33</v>
       </c>
-      <c r="I17" s="2">
-        <f t="shared" si="1"/>
+      <c r="I17" s="3">
+        <f t="shared" si="3"/>
         <v>33.33</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="3">
         <v>33.33</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" s="3">
         <v>33.33</v>
       </c>
-      <c r="L17" s="2">
-        <f t="shared" si="2"/>
+      <c r="L17" s="3">
+        <f t="shared" si="4"/>
         <v>33.33</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>18</v>
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B18" s="2">
         <v>20</v>
@@ -1354,21 +1400,21 @@
       <c r="D18" s="2">
         <v>75</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="2">
         <v>50</v>
       </c>
       <c r="F18" s="3">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="2">
         <v>25</v>
       </c>
       <c r="H18" s="2">
         <v>25</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="J18" s="2">
@@ -1378,13 +1424,13 @@
         <v>25</v>
       </c>
       <c r="L18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>19</v>
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B19" s="2">
         <v>224</v>
@@ -1395,21 +1441,21 @@
       <c r="D19" s="2">
         <v>75</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="2">
         <v>75</v>
       </c>
       <c r="F19" s="3">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="2">
         <v>50</v>
       </c>
       <c r="H19" s="2">
         <v>50</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="J19" s="2">
@@ -1419,13 +1465,13 @@
         <v>50</v>
       </c>
       <c r="L19" s="2">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
-        <v>20</v>
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B20" s="2">
         <v>140</v>
@@ -1433,40 +1479,40 @@
       <c r="C20" s="2">
         <v>10</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="3">
         <v>68.78</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>65.959999999999994</v>
       </c>
       <c r="F20" s="3">
         <f t="shared" si="0"/>
         <v>67.340489832269554</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="2">
         <v>48</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="3">
         <v>42.5</v>
       </c>
-      <c r="I20" s="2">
-        <f t="shared" si="1"/>
+      <c r="I20" s="3">
+        <f t="shared" si="3"/>
         <v>45.082872928176798</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="3">
         <v>50.33</v>
       </c>
-      <c r="K20" s="2">
+      <c r="K20" s="3">
         <v>47.5</v>
       </c>
-      <c r="L20" s="2">
-        <f t="shared" si="2"/>
+      <c r="L20" s="3">
+        <f t="shared" si="4"/>
         <v>48.874067259531834</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
-        <v>21</v>
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="2">
         <v>376</v>
@@ -1477,21 +1523,21 @@
       <c r="D21" s="2">
         <v>50</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="2">
         <v>50</v>
       </c>
       <c r="F21" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="2">
         <v>25</v>
       </c>
       <c r="H21" s="2">
         <v>25</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="J21" s="2">
@@ -1501,13 +1547,13 @@
         <v>25</v>
       </c>
       <c r="L21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
-        <v>22</v>
+    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B22" s="2">
         <v>3580</v>
@@ -1515,40 +1561,40 @@
       <c r="C22" s="2">
         <v>9</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="3">
         <v>56.89</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="3">
         <v>51.66</v>
       </c>
       <c r="F22" s="3">
         <f t="shared" si="0"/>
         <v>54.149007830492856</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="3">
         <v>43.18</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <v>42.5</v>
       </c>
-      <c r="I22" s="2">
-        <f t="shared" si="1"/>
+      <c r="I22" s="3">
+        <f t="shared" si="3"/>
         <v>42.837301587301589</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="3">
         <v>54.31</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="3">
         <v>50.63</v>
       </c>
-      <c r="L22" s="2">
-        <f t="shared" si="2"/>
+      <c r="L22" s="3">
+        <f t="shared" si="4"/>
         <v>52.40547550981514</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
-        <v>23</v>
+    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B23" s="2">
         <v>178</v>
@@ -1559,21 +1605,21 @@
       <c r="D23" s="2">
         <v>100</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="2">
         <v>100</v>
       </c>
       <c r="F23" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="2">
         <v>100</v>
       </c>
       <c r="H23" s="2">
         <v>75</v>
       </c>
-      <c r="I23" s="2">
-        <f t="shared" si="1"/>
+      <c r="I23" s="3">
+        <f t="shared" si="3"/>
         <v>85.714285714285708</v>
       </c>
       <c r="J23" s="2">
@@ -1583,13 +1629,13 @@
         <v>100</v>
       </c>
       <c r="L23" s="2">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
-        <v>24</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B24" s="2">
         <v>304</v>
@@ -1600,21 +1646,21 @@
       <c r="D24" s="2">
         <v>100</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="2">
         <v>100</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="2">
         <v>100</v>
       </c>
       <c r="H24" s="2">
         <v>75</v>
       </c>
-      <c r="I24" s="2">
-        <f t="shared" si="1"/>
+      <c r="I24" s="3">
+        <f t="shared" si="3"/>
         <v>85.714285714285708</v>
       </c>
       <c r="J24" s="2">
@@ -1624,13 +1670,13 @@
         <v>100</v>
       </c>
       <c r="L24" s="2">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>25</v>
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B25" s="2">
         <v>25000</v>
@@ -1638,40 +1684,40 @@
       <c r="C25" s="2">
         <v>62</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="3">
         <v>67.06</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="3">
         <v>62.41</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="0"/>
         <v>64.651496099482515</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="3">
         <v>49.19</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="3">
         <v>42.87</v>
       </c>
-      <c r="I25" s="2">
-        <f t="shared" si="1"/>
+      <c r="I25" s="3">
+        <f t="shared" si="3"/>
         <v>45.813063219639361</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="3">
         <v>56.72</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="3">
         <v>56.37</v>
       </c>
-      <c r="L25" s="2">
-        <f t="shared" si="2"/>
+      <c r="L25" s="3">
+        <f t="shared" si="4"/>
         <v>56.544458395967808</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>26</v>
+    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B26" s="2">
         <v>6050</v>
@@ -1682,37 +1728,37 @@
       <c r="D26" s="2">
         <v>65</v>
       </c>
-      <c r="E26" s="1">
+      <c r="E26" s="3">
         <v>67.55</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="0"/>
         <v>66.250471520181051</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G26" s="3">
         <v>55.33</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <v>47.22</v>
       </c>
-      <c r="I26" s="2">
-        <f t="shared" si="1"/>
+      <c r="I26" s="3">
+        <f t="shared" si="3"/>
         <v>50.954316918576296</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="3">
         <v>60.88</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="3">
         <v>51.66</v>
       </c>
-      <c r="L26" s="2">
-        <f t="shared" si="2"/>
+      <c r="L26" s="3">
+        <f t="shared" si="4"/>
         <v>55.892319175404303</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>27</v>
+    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B27" s="2">
         <v>464</v>
@@ -1723,21 +1769,21 @@
       <c r="D27" s="2">
         <v>50</v>
       </c>
-      <c r="E27" s="1">
+      <c r="E27" s="2">
         <v>50</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="2">
         <v>50</v>
       </c>
       <c r="H27" s="2">
         <v>50</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>50</v>
       </c>
       <c r="J27" s="2">
@@ -1747,13 +1793,13 @@
         <v>50</v>
       </c>
       <c r="L27" s="2">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>28</v>
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B28" s="2">
         <v>1680</v>
@@ -1761,40 +1807,40 @@
       <c r="C28" s="2">
         <v>4</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="3">
         <v>55.4</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E28" s="3">
         <v>52.5</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="0"/>
         <v>53.911028730305837</v>
       </c>
-      <c r="G28" s="1">
+      <c r="G28" s="3">
         <v>53.63</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="3">
         <v>45.47</v>
       </c>
-      <c r="I28" s="2">
-        <f t="shared" si="1"/>
+      <c r="I28" s="3">
+        <f t="shared" si="3"/>
         <v>49.214048435923317</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="3">
         <v>54.9</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="3">
         <v>52.2</v>
       </c>
-      <c r="L28" s="2">
-        <f t="shared" si="2"/>
+      <c r="L28" s="3">
+        <f t="shared" si="4"/>
         <v>53.515966386554631</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>29</v>
+    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B29" s="2">
         <v>472</v>
@@ -1805,37 +1851,37 @@
       <c r="D29" s="2">
         <v>50</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="2">
         <v>50</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="G29" s="1">
-        <v>50</v>
-      </c>
-      <c r="H29" s="1">
+      <c r="G29" s="2">
+        <v>50</v>
+      </c>
+      <c r="H29" s="2">
         <v>50</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="1"/>
-        <v>50</v>
-      </c>
-      <c r="J29" s="1">
-        <v>50</v>
-      </c>
-      <c r="K29" s="1">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="J29" s="2">
+        <v>50</v>
+      </c>
+      <c r="K29" s="2">
         <v>50</v>
       </c>
       <c r="L29" s="2">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>30</v>
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B30" s="2">
         <v>1710</v>
@@ -1843,40 +1889,40 @@
       <c r="C30" s="2">
         <v>4</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="3">
         <v>55.2</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E30" s="3">
         <v>52.5</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="0"/>
         <v>53.816155988857936</v>
       </c>
-      <c r="G30" s="1">
+      <c r="G30" s="3">
         <v>50.2</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="3">
         <v>47.5</v>
       </c>
-      <c r="I30" s="2">
-        <f t="shared" si="1"/>
+      <c r="I30" s="3">
+        <f t="shared" si="3"/>
         <v>48.812691914022516</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="3">
         <v>50.2</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="3">
         <v>47.5</v>
       </c>
-      <c r="L30" s="2">
-        <f t="shared" si="2"/>
+      <c r="L30" s="3">
+        <f t="shared" si="4"/>
         <v>48.812691914022516</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>31</v>
+    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="B31" s="2">
         <v>45500</v>
@@ -1884,40 +1930,40 @@
       <c r="C31" s="2">
         <v>80</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="3">
         <v>62.1</v>
       </c>
-      <c r="E31" s="1">
+      <c r="E31" s="3">
         <v>60.89</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="0"/>
         <v>61.489047890072364</v>
       </c>
-      <c r="G31" s="1">
+      <c r="G31" s="3">
         <v>53.33</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="3">
         <v>39.56</v>
       </c>
-      <c r="I31" s="2">
-        <f t="shared" si="1"/>
+      <c r="I31" s="3">
+        <f t="shared" si="3"/>
         <v>45.42436860803101</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="3">
         <v>62.5</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="3">
         <v>60.29</v>
       </c>
-      <c r="L31" s="2">
-        <f t="shared" si="2"/>
+      <c r="L31" s="3">
+        <f t="shared" si="4"/>
         <v>61.375111979802917</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>32</v>
+    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="B32" s="2">
         <v>380</v>
@@ -1928,13 +1974,13 @@
       <c r="D32" s="2">
         <v>0</v>
       </c>
-      <c r="E32" s="1">
+      <c r="E32" s="2">
         <v>0</v>
       </c>
       <c r="F32" s="3">
         <v>0</v>
       </c>
-      <c r="G32" s="1">
+      <c r="G32" s="2">
         <v>0</v>
       </c>
       <c r="H32" s="2">
@@ -1953,9 +1999,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
-        <v>33</v>
+    <row r="33" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="B33" s="2">
         <v>44</v>
@@ -1966,21 +2012,21 @@
       <c r="D33" s="2">
         <v>100</v>
       </c>
-      <c r="E33" s="1">
+      <c r="E33" s="2">
         <v>100</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G33" s="1">
+        <f>2*(D33*E33)/(D33+E33)</f>
+        <v>100</v>
+      </c>
+      <c r="G33" s="2">
         <v>100</v>
       </c>
       <c r="H33" s="2">
         <v>100</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="1"/>
+        <f>2*(G33*H33)/(G33+H33)</f>
         <v>100</v>
       </c>
       <c r="J33" s="2">
@@ -1990,13 +2036,13 @@
         <v>100</v>
       </c>
       <c r="L33" s="2">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
-        <v>34</v>
+        <f>2*(J33*K33)/(J33+K33)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>44</v>
       </c>
       <c r="B34" s="2">
         <v>9320</v>
@@ -2007,37 +2053,37 @@
       <c r="D34" s="2">
         <v>63</v>
       </c>
-      <c r="E34" s="1">
+      <c r="E34" s="3">
         <v>65.55</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="0"/>
+        <f>2*(D34*E34)/(D34+E34)</f>
         <v>64.249708284714103</v>
       </c>
-      <c r="G34" s="1">
+      <c r="G34" s="3">
         <v>53.33</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="3">
         <v>45.22</v>
       </c>
-      <c r="I34" s="2">
-        <f t="shared" si="1"/>
+      <c r="I34" s="3">
+        <f>2*(G34*H34)/(G34+H34)</f>
         <v>48.941300862506338</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="3">
         <v>58.88</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="3">
         <v>49.66</v>
       </c>
-      <c r="L34" s="2">
-        <f t="shared" si="2"/>
+      <c r="L34" s="3">
+        <f>2*(J34*K34)/(J34+K34)</f>
         <v>53.878400589644372</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
-        <v>35</v>
+    <row r="35" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B35" s="2">
         <v>1800</v>
@@ -2045,40 +2091,40 @@
       <c r="C35" s="2">
         <v>5</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="3">
         <v>66.72</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="3">
         <v>61.55</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="0"/>
+        <f>2*(D35*E35)/(D35+E35)</f>
         <v>64.030810010134886</v>
       </c>
-      <c r="G35" s="1">
+      <c r="G35" s="3">
         <v>52.4</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="3">
         <v>40.75</v>
       </c>
-      <c r="I35" s="2">
-        <f t="shared" si="1"/>
+      <c r="I35" s="3">
+        <f>2*(G35*H35)/(G35+H35)</f>
         <v>45.846484165324739</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="3">
         <v>64.599999999999994</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="3">
         <v>58.2</v>
       </c>
-      <c r="L35" s="2">
-        <f t="shared" si="2"/>
+      <c r="L35" s="3">
+        <f>2*(J35*K35)/(J35+K35)</f>
         <v>61.233224755700327</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
-        <v>36</v>
+    <row r="36" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="B36" s="2">
         <v>144</v>
@@ -2089,13 +2135,13 @@
       <c r="D36" s="2">
         <v>0</v>
       </c>
-      <c r="E36" s="1">
+      <c r="E36" s="2">
         <v>0</v>
       </c>
       <c r="F36" s="3">
         <v>0</v>
       </c>
-      <c r="G36" s="1">
+      <c r="G36" s="2">
         <v>0</v>
       </c>
       <c r="H36" s="2">
@@ -2114,9 +2160,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
-        <v>37</v>
+    <row r="37" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
       </c>
       <c r="B37" s="2">
         <v>1990</v>
@@ -2124,40 +2170,40 @@
       <c r="C37" s="2">
         <v>6</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="3">
         <v>65.5</v>
       </c>
-      <c r="E37" s="1">
+      <c r="E37" s="3">
         <v>60.55</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F37:F48" si="5">2*(D37*E37)/(D37+E37)</f>
         <v>62.927806426021412</v>
       </c>
-      <c r="G37" s="1">
+      <c r="G37" s="3">
         <v>50.2</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="3">
         <v>41.62</v>
       </c>
-      <c r="I37" s="2">
-        <f t="shared" si="1"/>
+      <c r="I37" s="3">
+        <f t="shared" ref="I37:I48" si="6">2*(G37*H37)/(G37+H37)</f>
         <v>45.509126551949471</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="3">
         <v>65.2</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="3">
         <v>58.5</v>
       </c>
-      <c r="L37" s="2">
-        <f t="shared" si="2"/>
+      <c r="L37" s="3">
+        <f t="shared" ref="L37:L48" si="7">2*(J37*K37)/(J37+K37)</f>
         <v>61.66855295068715</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
-        <v>38</v>
+    <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>48</v>
       </c>
       <c r="B38" s="2">
         <v>28700</v>
@@ -2165,40 +2211,40 @@
       <c r="C38" s="2">
         <v>65</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="3">
         <v>69.58</v>
       </c>
-      <c r="E38" s="1">
+      <c r="E38" s="3">
         <v>65.92</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>67.700569741697421</v>
       </c>
-      <c r="G38" s="1">
+      <c r="G38" s="3">
         <v>46.41</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="3">
         <v>40.69</v>
       </c>
-      <c r="I38" s="2">
-        <f t="shared" si="1"/>
+      <c r="I38" s="3">
+        <f t="shared" si="6"/>
         <v>43.362179104477612</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="3">
         <v>50.64</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="3">
         <v>43.02</v>
       </c>
-      <c r="L38" s="2">
-        <f t="shared" si="2"/>
+      <c r="L38" s="3">
+        <f t="shared" si="7"/>
         <v>46.520025624599626</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
-        <v>39</v>
+    <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="B39" s="2">
         <v>3700</v>
@@ -2206,40 +2252,40 @@
       <c r="C39" s="2">
         <v>11</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="3">
         <v>46.21</v>
       </c>
-      <c r="E39" s="1">
+      <c r="E39" s="3">
         <v>41.66</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>43.81719813360646</v>
       </c>
-      <c r="G39" s="1">
+      <c r="G39" s="3">
         <v>30.3</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="3">
         <v>26.51</v>
       </c>
-      <c r="I39" s="2">
-        <f t="shared" si="1"/>
+      <c r="I39" s="3">
+        <f t="shared" si="6"/>
         <v>28.278577715190988</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="3">
         <v>27.27</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="3">
         <v>22.72</v>
       </c>
-      <c r="L39" s="2">
-        <f t="shared" si="2"/>
+      <c r="L39" s="3">
+        <f t="shared" si="7"/>
         <v>24.787933586717344</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
-        <v>40</v>
+    <row r="40" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="B40" s="2">
         <v>7410</v>
@@ -2247,40 +2293,40 @@
       <c r="C40" s="2">
         <v>21</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="3">
         <v>65.7</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E40" s="3">
         <v>62.5</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>64.060062402496101</v>
       </c>
-      <c r="G40" s="1">
+      <c r="G40" s="3">
         <v>48.5</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="3">
         <v>43.2</v>
       </c>
-      <c r="I40" s="2">
-        <f t="shared" si="1"/>
+      <c r="I40" s="3">
+        <f t="shared" si="6"/>
         <v>45.696837513631408</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="3">
         <v>60.5</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="3">
         <v>57.33</v>
       </c>
-      <c r="L40" s="2">
-        <f t="shared" si="2"/>
+      <c r="L40" s="3">
+        <f t="shared" si="7"/>
         <v>58.872358482559612</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
-        <v>41</v>
+    <row r="41" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="B41" s="2">
         <v>5680</v>
@@ -2288,40 +2334,40 @@
       <c r="C41" s="2">
         <v>12</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="3">
         <v>63.78</v>
       </c>
-      <c r="E41" s="1">
+      <c r="E41" s="3">
         <v>60.55</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>62.123043513230918</v>
       </c>
-      <c r="G41" s="1">
+      <c r="G41" s="3">
         <v>50.33</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="3">
         <v>46.22</v>
       </c>
-      <c r="I41" s="2">
-        <f t="shared" si="1"/>
+      <c r="I41" s="3">
+        <f t="shared" si="6"/>
         <v>48.1875214914552</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="3">
         <v>59.88</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="3">
         <v>50.66</v>
       </c>
-      <c r="L41" s="2">
-        <f t="shared" si="2"/>
+      <c r="L41" s="3">
+        <f t="shared" si="7"/>
         <v>54.885485796996562</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
-        <v>42</v>
+    <row r="42" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="B42" s="2">
         <v>2100</v>
@@ -2329,40 +2375,40 @@
       <c r="C42" s="2">
         <v>6</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="3">
         <v>66.5</v>
       </c>
-      <c r="E42" s="1">
+      <c r="E42" s="3">
         <v>62.55</v>
       </c>
       <c r="F42" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>64.464548624564117</v>
       </c>
-      <c r="G42" s="1">
+      <c r="G42" s="3">
         <v>50.2</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="3">
         <v>45.62</v>
       </c>
-      <c r="I42" s="2">
-        <f t="shared" si="1"/>
+      <c r="I42" s="3">
+        <f t="shared" si="6"/>
         <v>47.800542684199542</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="3">
         <v>65.7</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="3">
         <v>52.66</v>
       </c>
-      <c r="L42" s="2">
-        <f t="shared" si="2"/>
+      <c r="L42" s="3">
+        <f t="shared" si="7"/>
         <v>58.461676241973635</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
-        <v>43</v>
+    <row r="43" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>53</v>
       </c>
       <c r="B43" s="2">
         <v>5860</v>
@@ -2370,40 +2416,40 @@
       <c r="C43" s="2">
         <v>16</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43" s="3">
         <v>74.41</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E43" s="3">
         <v>70.22</v>
       </c>
       <c r="F43" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>72.254306851967087</v>
       </c>
-      <c r="G43" s="1">
+      <c r="G43" s="3">
         <v>67.84</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="3">
         <v>60.09</v>
       </c>
-      <c r="I43" s="2">
-        <f t="shared" si="1"/>
+      <c r="I43" s="3">
+        <f t="shared" si="6"/>
         <v>63.730252481826</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="3">
         <v>71.63</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="3">
         <v>64.87</v>
       </c>
-      <c r="L43" s="2">
-        <f t="shared" si="2"/>
+      <c r="L43" s="3">
+        <f t="shared" si="7"/>
         <v>68.082609523809523</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
-        <v>44</v>
+    <row r="44" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="B44" s="2">
         <v>2570</v>
@@ -2411,40 +2457,40 @@
       <c r="C44" s="2">
         <v>7</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44" s="3">
         <v>63.7</v>
       </c>
-      <c r="E44" s="1">
+      <c r="E44" s="2">
         <v>66</v>
       </c>
       <c r="F44" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>64.829606784888213</v>
       </c>
-      <c r="G44" s="1">
+      <c r="G44" s="3">
         <v>50.41</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="3">
         <v>45.69</v>
       </c>
-      <c r="I44" s="2">
-        <f t="shared" si="1"/>
+      <c r="I44" s="3">
+        <f t="shared" si="6"/>
         <v>47.934087408949004</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="3">
         <v>55.64</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="3">
         <v>55.66</v>
       </c>
-      <c r="L44" s="2">
-        <f t="shared" si="2"/>
+      <c r="L44" s="3">
+        <f t="shared" si="7"/>
         <v>55.649998203054807</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
-        <v>45</v>
+    <row r="45" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="B45" s="2">
         <v>768</v>
@@ -2455,21 +2501,21 @@
       <c r="D45" s="2">
         <v>50</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E45" s="2">
         <v>50</v>
       </c>
       <c r="F45" s="3">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="G45" s="1">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="G45" s="2">
         <v>50</v>
       </c>
       <c r="H45" s="2">
         <v>50</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="J45" s="2">
@@ -2479,13 +2525,13 @@
         <v>50</v>
       </c>
       <c r="L45" s="2">
-        <f t="shared" si="2"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
-        <v>46</v>
+        <f t="shared" si="7"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>56</v>
       </c>
       <c r="B46" s="2">
         <v>788</v>
@@ -2496,21 +2542,21 @@
       <c r="D46" s="2">
         <v>75</v>
       </c>
-      <c r="E46" s="1">
+      <c r="E46" s="2">
         <v>75</v>
       </c>
       <c r="F46" s="3">
-        <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="G46" s="1">
+        <f t="shared" si="5"/>
+        <v>75</v>
+      </c>
+      <c r="G46" s="2">
         <v>75</v>
       </c>
       <c r="H46" s="2">
         <v>75</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>75</v>
       </c>
       <c r="J46" s="2">
@@ -2520,13 +2566,13 @@
         <v>75</v>
       </c>
       <c r="L46" s="2">
-        <f t="shared" si="2"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
-        <v>47</v>
+        <f t="shared" si="7"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="B47" s="2">
         <v>2850</v>
@@ -2537,37 +2583,37 @@
       <c r="D47" s="2">
         <v>74</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="3">
         <v>69.66</v>
       </c>
       <c r="F47" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>71.764443825699573</v>
       </c>
-      <c r="G47" s="1">
+      <c r="G47" s="3">
         <v>69.84</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="3">
         <v>64.09</v>
       </c>
-      <c r="I47" s="2">
-        <f t="shared" si="1"/>
+      <c r="I47" s="3">
+        <f t="shared" si="6"/>
         <v>66.841567983274842</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J47" s="3">
         <v>70.63</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="3">
         <v>66.5</v>
       </c>
-      <c r="L47" s="2">
-        <f t="shared" si="2"/>
+      <c r="L47" s="3">
+        <f t="shared" si="7"/>
         <v>68.502807554874934</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
-        <v>48</v>
+    <row r="48" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>58</v>
       </c>
       <c r="B48" s="2">
         <v>36</v>
@@ -2578,21 +2624,21 @@
       <c r="D48" s="2">
         <v>100</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="2">
         <v>100</v>
       </c>
       <c r="F48" s="3">
-        <f t="shared" si="0"/>
-        <v>100</v>
-      </c>
-      <c r="G48" s="1">
+        <f t="shared" si="5"/>
+        <v>100</v>
+      </c>
+      <c r="G48" s="2">
         <v>100</v>
       </c>
       <c r="H48" s="2">
         <v>100</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="6"/>
         <v>100</v>
       </c>
       <c r="J48" s="2">
@@ -2602,13 +2648,13 @@
         <v>100</v>
       </c>
       <c r="L48" s="2">
-        <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
-        <v>49</v>
+        <f t="shared" si="7"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="B49" s="2">
         <v>148</v>
@@ -2619,13 +2665,13 @@
       <c r="D49" s="2">
         <v>0</v>
       </c>
-      <c r="E49" s="1">
+      <c r="E49" s="2">
         <v>0</v>
       </c>
       <c r="F49" s="3">
         <v>0</v>
       </c>
-      <c r="G49" s="1">
+      <c r="G49" s="2">
         <v>0</v>
       </c>
       <c r="H49" s="2">
@@ -2644,9 +2690,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
-        <v>50</v>
+    <row r="50" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>60</v>
       </c>
       <c r="B50" s="2">
         <v>3120</v>
@@ -2654,40 +2700,40 @@
       <c r="C50" s="2">
         <v>8</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="3">
         <v>63.5</v>
       </c>
-      <c r="E50" s="1">
+      <c r="E50" s="3">
         <v>55.2</v>
       </c>
       <c r="F50" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F50:F62" si="8">2*(D50*E50)/(D50+E50)</f>
         <v>59.05981465880371</v>
       </c>
-      <c r="G50" s="1">
+      <c r="G50" s="3">
         <v>52.1</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="3">
         <v>45.5</v>
       </c>
-      <c r="I50" s="2">
-        <f t="shared" si="1"/>
+      <c r="I50" s="3">
+        <f t="shared" ref="I50:I62" si="9">2*(G50*H50)/(G50+H50)</f>
         <v>48.57684426229509</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J50" s="3">
         <v>58.5</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K50" s="3">
         <v>55.3</v>
       </c>
-      <c r="L50" s="2">
-        <f>2*(J50*K50)/(J50+K50)</f>
+      <c r="L50" s="3">
+        <f t="shared" ref="L50:L62" si="10">2*(J50*K50)/(J50+K50)</f>
         <v>56.855008787346215</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>51</v>
+    <row r="51" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>61</v>
       </c>
       <c r="B51" s="2">
         <v>2680</v>
@@ -2698,37 +2744,37 @@
       <c r="D51" s="2">
         <v>50</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E51" s="2">
         <v>50</v>
       </c>
       <c r="F51" s="3">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="G51" s="1">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="G51" s="2">
         <v>58</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="3">
         <v>48.8</v>
       </c>
-      <c r="I51" s="2">
-        <f t="shared" si="1"/>
+      <c r="I51" s="3">
+        <f t="shared" si="9"/>
         <v>53.003745318352053</v>
       </c>
-      <c r="J51" s="2">
+      <c r="J51" s="3">
         <v>42.85</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K51" s="3">
         <v>38.090000000000003</v>
       </c>
-      <c r="L51" s="2">
-        <f t="shared" si="2"/>
+      <c r="L51" s="3">
+        <f t="shared" si="10"/>
         <v>40.330034593526079</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A52" s="2" t="s">
-        <v>52</v>
+    <row r="52" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>62</v>
       </c>
       <c r="B52" s="2">
         <v>2980</v>
@@ -2736,40 +2782,40 @@
       <c r="C52" s="2">
         <v>9</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52" s="3">
         <v>60.5</v>
       </c>
-      <c r="E52" s="1">
+      <c r="E52" s="3">
         <v>55.33</v>
       </c>
       <c r="F52" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="8"/>
         <v>57.799620132953464</v>
       </c>
-      <c r="G52" s="1">
+      <c r="G52" s="3">
         <v>45.25</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="3">
         <v>40.5</v>
       </c>
-      <c r="I52" s="2">
-        <f t="shared" si="1"/>
+      <c r="I52" s="3">
+        <f t="shared" si="9"/>
         <v>42.74344023323615</v>
       </c>
-      <c r="J52" s="2">
+      <c r="J52" s="3">
         <v>50.4</v>
       </c>
-      <c r="K52" s="2">
+      <c r="K52" s="3">
         <v>48.65</v>
       </c>
-      <c r="L52" s="2">
-        <f t="shared" si="2"/>
+      <c r="L52" s="3">
+        <f t="shared" si="10"/>
         <v>49.509540636042402</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A53" s="2" t="s">
-        <v>53</v>
+    <row r="53" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>63</v>
       </c>
       <c r="B53" s="2">
         <v>408</v>
@@ -2780,21 +2826,21 @@
       <c r="D53" s="2">
         <v>50</v>
       </c>
-      <c r="E53" s="1">
+      <c r="E53" s="2">
         <v>50</v>
       </c>
       <c r="F53" s="3">
-        <f t="shared" ref="F53:F78" si="3">2*(D53*E53)/(D53+E53)</f>
-        <v>50</v>
-      </c>
-      <c r="G53" s="1">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="G53" s="2">
         <v>50</v>
       </c>
       <c r="H53" s="2">
         <v>50</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" ref="I53:I80" si="4">2*(G53*H53)/(G53+H53)</f>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="J53" s="2">
@@ -2804,13 +2850,13 @@
         <v>50</v>
       </c>
       <c r="L53" s="2">
-        <f t="shared" ref="L53:L80" si="5">2*(J53*K53)/(J53+K53)</f>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A54" s="2" t="s">
-        <v>54</v>
+        <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="B54" s="2">
         <v>32</v>
@@ -2821,21 +2867,21 @@
       <c r="D54" s="2">
         <v>50</v>
       </c>
-      <c r="E54" s="1">
+      <c r="E54" s="2">
         <v>50</v>
       </c>
       <c r="F54" s="3">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="G54" s="1">
+        <f t="shared" si="8"/>
+        <v>50</v>
+      </c>
+      <c r="G54" s="2">
         <v>50</v>
       </c>
       <c r="H54" s="2">
         <v>50</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>50</v>
       </c>
       <c r="J54" s="2">
@@ -2845,13 +2891,13 @@
         <v>50</v>
       </c>
       <c r="L54" s="2">
-        <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="2" t="s">
-        <v>55</v>
+        <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="B55" s="2">
         <v>332</v>
@@ -2862,21 +2908,21 @@
       <c r="D55" s="2">
         <v>100</v>
       </c>
-      <c r="E55" s="1">
+      <c r="E55" s="2">
         <v>100</v>
       </c>
       <c r="F55" s="3">
-        <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-      <c r="G55" s="1">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="G55" s="2">
         <v>25</v>
       </c>
       <c r="H55" s="2">
         <v>25</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="J55" s="2">
@@ -2886,13 +2932,13 @@
         <v>25</v>
       </c>
       <c r="L55" s="2">
-        <f>2*(J55*K55)/(J55+K55)</f>
+        <f t="shared" si="10"/>
         <v>25</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A56" s="2" t="s">
-        <v>56</v>
+    <row r="56" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="B56" s="2">
         <v>1570</v>
@@ -2903,21 +2949,21 @@
       <c r="D56" s="2">
         <v>75</v>
       </c>
-      <c r="E56" s="1">
+      <c r="E56" s="2">
         <v>75</v>
       </c>
       <c r="F56" s="3">
-        <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="G56" s="1">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="G56" s="2">
         <v>75</v>
       </c>
       <c r="H56" s="2">
         <v>75</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>75</v>
       </c>
       <c r="J56" s="2">
@@ -2927,13 +2973,13 @@
         <v>50</v>
       </c>
       <c r="L56" s="2">
-        <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A57" s="2" t="s">
-        <v>57</v>
+        <f t="shared" si="10"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="B57" s="2">
         <v>240</v>
@@ -2944,37 +2990,37 @@
       <c r="D57" s="2">
         <v>75</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="2">
         <v>75</v>
       </c>
       <c r="F57" s="3">
-        <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="G57" s="1">
-        <v>50</v>
-      </c>
-      <c r="H57" s="1">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="G57" s="2">
+        <v>50</v>
+      </c>
+      <c r="H57" s="2">
         <v>50</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" si="4"/>
-        <v>50</v>
-      </c>
-      <c r="J57" s="1">
-        <v>75</v>
-      </c>
-      <c r="K57" s="1">
+        <f t="shared" si="9"/>
+        <v>50</v>
+      </c>
+      <c r="J57" s="2">
+        <v>75</v>
+      </c>
+      <c r="K57" s="2">
         <v>75</v>
       </c>
       <c r="L57" s="2">
-        <f t="shared" si="5"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A58" s="2" t="s">
-        <v>58</v>
+        <f t="shared" si="10"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="B58" s="2">
         <v>1790</v>
@@ -2982,24 +3028,24 @@
       <c r="C58" s="2">
         <v>5</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58" s="3">
         <v>68.5</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E58" s="3">
         <v>65.55</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>66.992540096978743</v>
       </c>
-      <c r="G58" s="1">
+      <c r="G58" s="3">
         <v>50.2</v>
       </c>
-      <c r="H58" s="2">
+      <c r="H58" s="3">
         <v>42.62</v>
       </c>
-      <c r="I58" s="2">
-        <f t="shared" si="4"/>
+      <c r="I58" s="3">
+        <f t="shared" si="9"/>
         <v>46.100495582848524</v>
       </c>
       <c r="J58" s="2">
@@ -3008,14 +3054,14 @@
       <c r="K58" s="2">
         <v>52</v>
       </c>
-      <c r="L58" s="2">
-        <f t="shared" si="5"/>
+      <c r="L58" s="3">
+        <f t="shared" si="10"/>
         <v>57.777777777777779</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A59" s="2" t="s">
-        <v>59</v>
+    <row r="59" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="B59" s="2">
         <v>6640</v>
@@ -3023,40 +3069,40 @@
       <c r="C59" s="2">
         <v>15</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59" s="3">
         <v>70.239999999999995</v>
       </c>
-      <c r="E59" s="1">
+      <c r="E59" s="3">
         <v>61.5</v>
       </c>
       <c r="F59" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>65.580081979656882</v>
       </c>
-      <c r="G59" s="1">
+      <c r="G59" s="3">
         <v>50.33</v>
       </c>
-      <c r="H59" s="2">
+      <c r="H59" s="3">
         <v>42.39</v>
       </c>
-      <c r="I59" s="2">
-        <f t="shared" si="4"/>
+      <c r="I59" s="3">
+        <f t="shared" si="9"/>
         <v>46.020032355478861</v>
       </c>
-      <c r="J59" s="2">
+      <c r="J59" s="3">
         <v>66.2</v>
       </c>
-      <c r="K59" s="2">
+      <c r="K59" s="3">
         <v>60.85</v>
       </c>
-      <c r="L59" s="2">
-        <f t="shared" si="5"/>
+      <c r="L59" s="3">
+        <f t="shared" si="10"/>
         <v>63.41235733963007</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A60" s="2" t="s">
-        <v>60</v>
+    <row r="60" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="B60" s="2">
         <v>372</v>
@@ -3067,21 +3113,21 @@
       <c r="D60" s="2">
         <v>75</v>
       </c>
-      <c r="E60" s="1">
+      <c r="E60" s="2">
         <v>75</v>
       </c>
       <c r="F60" s="3">
-        <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="G60" s="1">
+        <f t="shared" si="8"/>
+        <v>75</v>
+      </c>
+      <c r="G60" s="2">
         <v>75</v>
       </c>
       <c r="H60" s="2">
         <v>75</v>
       </c>
       <c r="I60" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>75</v>
       </c>
       <c r="J60" s="2">
@@ -3091,13 +3137,13 @@
         <v>75</v>
       </c>
       <c r="L60" s="2">
-        <f t="shared" si="5"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A61" s="2" t="s">
-        <v>61</v>
+        <f t="shared" si="10"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="B61" s="2">
         <v>240</v>
@@ -3105,40 +3151,40 @@
       <c r="C61" s="2">
         <v>5</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61" s="3">
         <v>62.5</v>
       </c>
-      <c r="E61" s="1">
+      <c r="E61" s="3">
         <v>61.25</v>
       </c>
       <c r="F61" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>61.868686868686872</v>
       </c>
-      <c r="G61" s="1">
+      <c r="G61" s="3">
         <v>53.98</v>
       </c>
-      <c r="H61" s="2">
+      <c r="H61" s="3">
         <v>48.04</v>
       </c>
-      <c r="I61" s="2">
-        <f t="shared" si="4"/>
+      <c r="I61" s="3">
+        <f t="shared" si="9"/>
         <v>50.837075083316996</v>
       </c>
-      <c r="J61" s="2">
+      <c r="J61" s="3">
         <v>58.59</v>
       </c>
-      <c r="K61" s="2">
+      <c r="K61" s="3">
         <v>55.61</v>
       </c>
-      <c r="L61" s="2">
-        <f t="shared" si="5"/>
+      <c r="L61" s="3">
+        <f t="shared" si="10"/>
         <v>57.061119089316989</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A62" s="2" t="s">
-        <v>62</v>
+    <row r="62" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="B62" s="2">
         <v>2270</v>
@@ -3146,40 +3192,40 @@
       <c r="C62" s="2">
         <v>6</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62" s="3">
         <v>72.709999999999994</v>
       </c>
-      <c r="E62" s="1">
+      <c r="E62" s="3">
         <v>69.52</v>
       </c>
       <c r="F62" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>71.079226604795053</v>
       </c>
-      <c r="G62" s="1">
+      <c r="G62" s="2">
         <v>52</v>
       </c>
-      <c r="H62" s="2">
+      <c r="H62" s="3">
         <v>47.52</v>
       </c>
-      <c r="I62" s="2">
-        <f t="shared" si="4"/>
+      <c r="I62" s="3">
+        <f t="shared" si="9"/>
         <v>49.659163987138257</v>
       </c>
-      <c r="J62" s="2">
+      <c r="J62" s="3">
         <v>68.5</v>
       </c>
-      <c r="K62" s="2">
+      <c r="K62" s="3">
         <v>65.66</v>
       </c>
-      <c r="L62" s="2">
-        <f t="shared" si="5"/>
+      <c r="L62" s="3">
+        <f t="shared" si="10"/>
         <v>67.049940369707812</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A63" s="2" t="s">
-        <v>63</v>
+    <row r="63" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>73</v>
       </c>
       <c r="B63" s="2">
         <v>32</v>
@@ -3190,13 +3236,13 @@
       <c r="D63" s="2">
         <v>0</v>
       </c>
-      <c r="E63" s="1">
+      <c r="E63" s="2">
         <v>0</v>
       </c>
       <c r="F63" s="3">
         <v>0</v>
       </c>
-      <c r="G63" s="1">
+      <c r="G63" s="2">
         <v>0</v>
       </c>
       <c r="H63" s="2">
@@ -3215,9 +3261,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A64" s="2" t="s">
-        <v>64</v>
+    <row r="64" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="B64" s="2">
         <v>20</v>
@@ -3225,40 +3271,40 @@
       <c r="C64" s="2">
         <v>3</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64" s="3">
         <v>70.25</v>
       </c>
-      <c r="E64" s="1">
+      <c r="E64" s="3">
         <v>56.36</v>
       </c>
       <c r="F64" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F64:F78" si="11">2*(D64*E64)/(D64+E64)</f>
         <v>62.543085064370899</v>
       </c>
-      <c r="G64" s="1">
+      <c r="G64" s="3">
         <v>47.75</v>
       </c>
-      <c r="H64" s="2">
+      <c r="H64" s="3">
         <v>42.33</v>
       </c>
-      <c r="I64" s="2">
-        <f t="shared" si="4"/>
+      <c r="I64" s="3">
+        <f t="shared" ref="I64:I80" si="12">2*(G64*H64)/(G64+H64)</f>
         <v>44.87694271758437</v>
       </c>
-      <c r="J64" s="2">
+      <c r="J64" s="3">
         <v>54.7</v>
       </c>
-      <c r="K64" s="2">
+      <c r="K64" s="3">
         <v>50.25</v>
       </c>
-      <c r="L64" s="2">
-        <f t="shared" si="5"/>
+      <c r="L64" s="3">
+        <f t="shared" ref="L64:L80" si="13">2*(J64*K64)/(J64+K64)</f>
         <v>52.380657455931399</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A65" s="2" t="s">
-        <v>65</v>
+    <row r="65" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="B65" s="2">
         <v>6320</v>
@@ -3266,40 +3312,40 @@
       <c r="C65" s="2">
         <v>20</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65" s="3">
         <v>68.540000000000006</v>
       </c>
-      <c r="E65" s="1">
+      <c r="E65" s="3">
         <v>65.39</v>
       </c>
       <c r="F65" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>66.927956395131787</v>
       </c>
-      <c r="G65" s="1">
+      <c r="G65" s="3">
         <v>50.25</v>
       </c>
-      <c r="H65" s="2">
+      <c r="H65" s="3">
         <v>47.2</v>
       </c>
-      <c r="I65" s="2">
-        <f t="shared" si="4"/>
+      <c r="I65" s="3">
+        <f t="shared" si="12"/>
         <v>48.677270395074402</v>
       </c>
-      <c r="J65" s="2">
+      <c r="J65" s="3">
         <v>65.319999999999993</v>
       </c>
-      <c r="K65" s="2">
+      <c r="K65" s="3">
         <v>63.1</v>
       </c>
-      <c r="L65" s="2">
-        <f t="shared" si="5"/>
+      <c r="L65" s="3">
+        <f t="shared" si="13"/>
         <v>64.190811400093452</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A66" s="2" t="s">
-        <v>66</v>
+    <row r="66" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="B66" s="2">
         <v>39800</v>
@@ -3307,40 +3353,40 @@
       <c r="C66" s="2">
         <v>78</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66" s="3">
         <v>62.13</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E66" s="3">
         <v>55.65</v>
       </c>
       <c r="F66" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>58.711742231278656</v>
       </c>
-      <c r="G66" s="1">
+      <c r="G66" s="3">
         <v>59.32</v>
       </c>
-      <c r="H66" s="2">
+      <c r="H66" s="3">
         <v>56.51</v>
       </c>
-      <c r="I66" s="2">
-        <f t="shared" si="4"/>
+      <c r="I66" s="3">
+        <f t="shared" si="12"/>
         <v>57.880915134248461</v>
       </c>
-      <c r="J66" s="2">
+      <c r="J66" s="3">
         <v>58.76</v>
       </c>
-      <c r="K66" s="2">
+      <c r="K66" s="3">
         <v>58.54</v>
       </c>
-      <c r="L66" s="2">
-        <f t="shared" si="5"/>
+      <c r="L66" s="3">
+        <f t="shared" si="13"/>
         <v>58.649793691389597</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A67" s="2" t="s">
-        <v>67</v>
+    <row r="67" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>77</v>
       </c>
       <c r="B67" s="2">
         <v>76</v>
@@ -3348,40 +3394,40 @@
       <c r="C67" s="2">
         <v>5</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67" s="3">
         <v>71.28</v>
       </c>
-      <c r="E67" s="1">
+      <c r="E67" s="3">
         <v>68.94</v>
       </c>
       <c r="F67" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>70.090474967907582</v>
       </c>
-      <c r="G67" s="1">
+      <c r="G67" s="3">
         <v>50.76</v>
       </c>
-      <c r="H67" s="2">
+      <c r="H67" s="3">
         <v>35.270000000000003</v>
       </c>
-      <c r="I67" s="2">
-        <f t="shared" si="4"/>
+      <c r="I67" s="3">
+        <f t="shared" si="12"/>
         <v>41.620485877019647</v>
       </c>
-      <c r="J67" s="2">
+      <c r="J67" s="3">
         <v>68.98</v>
       </c>
-      <c r="K67" s="2">
+      <c r="K67" s="3">
         <v>67.5</v>
       </c>
-      <c r="L67" s="2">
-        <f t="shared" si="5"/>
+      <c r="L67" s="3">
+        <f t="shared" si="13"/>
         <v>68.231975381008212</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A68" s="2" t="s">
-        <v>68</v>
+    <row r="68" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>78</v>
       </c>
       <c r="B68" s="2">
         <v>324</v>
@@ -3389,40 +3435,40 @@
       <c r="C68" s="2">
         <v>3</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68" s="3">
         <v>65.5</v>
       </c>
-      <c r="E68" s="1">
+      <c r="E68" s="2">
         <v>63</v>
       </c>
       <c r="F68" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>64.225680933852146</v>
       </c>
-      <c r="G68" s="1">
+      <c r="G68" s="2">
         <v>51</v>
       </c>
       <c r="H68" s="2">
         <v>45</v>
       </c>
-      <c r="I68" s="2">
-        <f t="shared" si="4"/>
+      <c r="I68" s="3">
+        <f t="shared" si="12"/>
         <v>47.8125</v>
       </c>
       <c r="J68" s="2">
         <v>64</v>
       </c>
-      <c r="K68" s="2">
+      <c r="K68" s="3">
         <v>58.83</v>
       </c>
-      <c r="L68" s="2">
-        <f t="shared" si="5"/>
+      <c r="L68" s="3">
+        <f t="shared" si="13"/>
         <v>61.306195554831881</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>69</v>
+    <row r="69" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>79</v>
       </c>
       <c r="B69" s="2">
         <v>24</v>
@@ -3433,21 +3479,21 @@
       <c r="D69" s="2">
         <v>75</v>
       </c>
-      <c r="E69" s="1">
+      <c r="E69" s="2">
         <v>75</v>
       </c>
       <c r="F69" s="3">
-        <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="G69" s="1">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="G69" s="2">
         <v>75</v>
       </c>
       <c r="H69" s="2">
         <v>75</v>
       </c>
       <c r="I69" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>75</v>
       </c>
       <c r="J69" s="2">
@@ -3457,13 +3503,13 @@
         <v>75</v>
       </c>
       <c r="L69" s="2">
-        <f t="shared" si="5"/>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>70</v>
+        <f t="shared" si="13"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>80</v>
       </c>
       <c r="B70" s="2">
         <v>396</v>
@@ -3474,37 +3520,37 @@
       <c r="D70" s="2">
         <v>75</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E70" s="3">
         <v>72.5</v>
       </c>
       <c r="F70" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>73.728813559322035</v>
       </c>
-      <c r="G70" s="1">
+      <c r="G70" s="3">
         <v>66.67</v>
       </c>
       <c r="H70" s="2">
         <v>64</v>
       </c>
-      <c r="I70" s="2">
-        <f t="shared" si="4"/>
+      <c r="I70" s="3">
+        <f t="shared" si="12"/>
         <v>65.307721741792292</v>
       </c>
       <c r="J70" s="2">
         <v>68</v>
       </c>
-      <c r="K70" s="2">
+      <c r="K70" s="3">
         <v>60.5</v>
       </c>
-      <c r="L70" s="2">
-        <f t="shared" si="5"/>
+      <c r="L70" s="3">
+        <f t="shared" si="13"/>
         <v>64.031128404669261</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A71" s="2" t="s">
-        <v>71</v>
+    <row r="71" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>81</v>
       </c>
       <c r="B71" s="2">
         <v>49500</v>
@@ -3512,40 +3558,40 @@
       <c r="C71" s="2">
         <v>150</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71" s="3">
         <v>50.94</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E71" s="3">
         <v>54.95</v>
       </c>
       <c r="F71" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>52.869071678156573</v>
       </c>
-      <c r="G71" s="1">
+      <c r="G71" s="3">
         <v>44.55</v>
       </c>
-      <c r="H71" s="2">
+      <c r="H71" s="3">
         <v>41.74</v>
       </c>
-      <c r="I71" s="2">
-        <f t="shared" si="4"/>
+      <c r="I71" s="3">
+        <f t="shared" si="12"/>
         <v>43.09924672615599</v>
       </c>
-      <c r="J71" s="2">
+      <c r="J71" s="3">
         <v>45.16</v>
       </c>
-      <c r="K71" s="2">
+      <c r="K71" s="3">
         <v>44.44</v>
       </c>
-      <c r="L71" s="2">
-        <f t="shared" si="5"/>
+      <c r="L71" s="3">
+        <f t="shared" si="13"/>
         <v>44.797107142857143</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
-        <v>72</v>
+    <row r="72" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="B72" s="2">
         <v>28</v>
@@ -3556,21 +3602,21 @@
       <c r="D72" s="2">
         <v>50</v>
       </c>
-      <c r="E72" s="1">
+      <c r="E72" s="2">
         <v>50</v>
       </c>
       <c r="F72" s="3">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="G72" s="1">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+      <c r="G72" s="2">
         <v>50</v>
       </c>
       <c r="H72" s="2">
         <v>50</v>
       </c>
       <c r="I72" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="J72" s="2">
@@ -3580,13 +3626,13 @@
         <v>50</v>
       </c>
       <c r="L72" s="2">
-        <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A73" s="2" t="s">
-        <v>73</v>
+        <f t="shared" si="13"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>83</v>
       </c>
       <c r="B73" s="2">
         <v>756</v>
@@ -3594,24 +3640,24 @@
       <c r="C73" s="2">
         <v>5</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73" s="3">
         <v>61.72</v>
       </c>
-      <c r="E73" s="1">
+      <c r="E73" s="3">
         <v>60.5</v>
       </c>
       <c r="F73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>61.103910980199643</v>
       </c>
-      <c r="G73" s="1">
+      <c r="G73" s="2">
         <v>58</v>
       </c>
       <c r="H73" s="2">
         <v>47</v>
       </c>
-      <c r="I73" s="2">
-        <f t="shared" si="4"/>
+      <c r="I73" s="3">
+        <f t="shared" si="12"/>
         <v>51.923809523809524</v>
       </c>
       <c r="J73" s="2">
@@ -3620,14 +3666,14 @@
       <c r="K73" s="2">
         <v>50</v>
       </c>
-      <c r="L73" s="2">
-        <f t="shared" si="5"/>
+      <c r="L73" s="3">
+        <f t="shared" si="13"/>
         <v>51.456310679611647</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A74" s="2" t="s">
-        <v>74</v>
+    <row r="74" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>84</v>
       </c>
       <c r="B74" s="2">
         <v>24</v>
@@ -3638,21 +3684,21 @@
       <c r="D74" s="2">
         <v>50</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E74" s="2">
         <v>50</v>
       </c>
       <c r="F74" s="3">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-      <c r="G74" s="1">
+        <f t="shared" si="11"/>
+        <v>50</v>
+      </c>
+      <c r="G74" s="2">
         <v>50</v>
       </c>
       <c r="H74" s="2">
         <v>50</v>
       </c>
       <c r="I74" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="J74" s="2">
@@ -3662,13 +3708,13 @@
         <v>50</v>
       </c>
       <c r="L74" s="2">
-        <f t="shared" si="5"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A75" s="2" t="s">
-        <v>75</v>
+        <f t="shared" si="13"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>85</v>
       </c>
       <c r="B75" s="2">
         <v>916</v>
@@ -3676,40 +3722,40 @@
       <c r="C75" s="2">
         <v>3</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75" s="3">
         <v>77.2</v>
       </c>
-      <c r="E75" s="1">
+      <c r="E75" s="3">
         <v>55.5</v>
       </c>
       <c r="F75" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>64.575734740015079</v>
       </c>
-      <c r="G75" s="1">
+      <c r="G75" s="2">
         <v>65</v>
       </c>
-      <c r="H75" s="2">
+      <c r="H75" s="3">
         <v>41.2</v>
       </c>
-      <c r="I75" s="2">
-        <f t="shared" si="4"/>
+      <c r="I75" s="3">
+        <f t="shared" si="12"/>
         <v>50.433145009416194</v>
       </c>
       <c r="J75" s="2">
         <v>62</v>
       </c>
-      <c r="K75" s="2">
+      <c r="K75" s="3">
         <v>59.5</v>
       </c>
-      <c r="L75" s="2">
-        <f t="shared" si="5"/>
+      <c r="L75" s="3">
+        <f t="shared" si="13"/>
         <v>60.724279835390945</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A76" s="2" t="s">
-        <v>76</v>
+    <row r="76" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="B76" s="2">
         <v>132</v>
@@ -3720,21 +3766,21 @@
       <c r="D76" s="2">
         <v>75</v>
       </c>
-      <c r="E76" s="1">
+      <c r="E76" s="2">
         <v>75</v>
       </c>
       <c r="F76" s="3">
-        <f t="shared" si="3"/>
-        <v>75</v>
-      </c>
-      <c r="G76" s="1">
+        <f t="shared" si="11"/>
+        <v>75</v>
+      </c>
+      <c r="G76" s="2">
         <v>75</v>
       </c>
       <c r="H76" s="2">
         <v>75</v>
       </c>
       <c r="I76" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>75</v>
       </c>
       <c r="J76" s="2">
@@ -3744,13 +3790,13 @@
         <v>100</v>
       </c>
       <c r="L76" s="2">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A77" s="2" t="s">
-        <v>77</v>
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="B77" s="2">
         <v>960</v>
@@ -3758,40 +3804,40 @@
       <c r="C77" s="2">
         <v>10</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77" s="3">
         <v>64.78</v>
       </c>
-      <c r="E77" s="1">
+      <c r="E77" s="3">
         <v>63.2</v>
       </c>
       <c r="F77" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>63.980246913580253</v>
       </c>
-      <c r="G77" s="1">
+      <c r="G77" s="3">
         <v>55.25</v>
       </c>
-      <c r="H77" s="2">
+      <c r="H77" s="3">
         <v>45.8</v>
       </c>
-      <c r="I77" s="2">
-        <f t="shared" si="4"/>
+      <c r="I77" s="3">
+        <f t="shared" si="12"/>
         <v>50.083127164769913</v>
       </c>
-      <c r="J77" s="2">
+      <c r="J77" s="3">
         <v>60.2</v>
       </c>
-      <c r="K77" s="2">
+      <c r="K77" s="3">
         <v>58.5</v>
       </c>
-      <c r="L77" s="2">
-        <f t="shared" si="5"/>
+      <c r="L77" s="3">
+        <f t="shared" si="13"/>
         <v>59.337826453243473</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A78" s="2" t="s">
-        <v>78</v>
+    <row r="78" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="B78" s="2">
         <v>596</v>
@@ -3802,37 +3848,37 @@
       <c r="D78" s="2">
         <v>65</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E78" s="3">
         <v>63.5</v>
       </c>
       <c r="F78" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="11"/>
         <v>64.241245136186777</v>
       </c>
-      <c r="G78" s="1">
-        <v>50</v>
-      </c>
-      <c r="H78" s="2">
+      <c r="G78" s="2">
+        <v>50</v>
+      </c>
+      <c r="H78" s="3">
         <v>46.8</v>
       </c>
-      <c r="I78" s="2">
-        <f t="shared" si="4"/>
+      <c r="I78" s="3">
+        <f t="shared" si="12"/>
         <v>48.347107438016529</v>
       </c>
-      <c r="J78" s="2">
+      <c r="J78" s="3">
         <v>64.8</v>
       </c>
-      <c r="K78" s="2">
+      <c r="K78" s="3">
         <v>63.1</v>
       </c>
-      <c r="L78" s="2">
-        <f t="shared" si="5"/>
+      <c r="L78" s="3">
+        <f t="shared" si="13"/>
         <v>63.938702111024234</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A79" s="2" t="s">
-        <v>79</v>
+    <row r="79" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="B79" s="2">
         <v>192</v>
@@ -3843,20 +3889,20 @@
       <c r="D79" s="2">
         <v>0</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E79" s="2">
         <v>0</v>
       </c>
       <c r="F79" s="3">
         <v>0</v>
       </c>
-      <c r="G79" s="1">
+      <c r="G79" s="2">
         <v>100</v>
       </c>
       <c r="H79" s="2">
         <v>100</v>
       </c>
       <c r="I79" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>100</v>
       </c>
       <c r="J79" s="2">
@@ -3866,13 +3912,13 @@
         <v>100</v>
       </c>
       <c r="L79" s="2">
-        <f t="shared" si="5"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A80" s="2" t="s">
-        <v>80</v>
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>90</v>
       </c>
       <c r="B80" s="2">
         <v>40</v>
@@ -3883,21 +3929,21 @@
       <c r="D80" s="2">
         <v>75</v>
       </c>
-      <c r="E80" s="1">
+      <c r="E80" s="2">
         <v>75</v>
       </c>
       <c r="F80" s="3">
         <f>2*(D80*E80)/(D80+E80)</f>
         <v>75</v>
       </c>
-      <c r="G80" s="1">
+      <c r="G80" s="2">
         <v>50</v>
       </c>
       <c r="H80" s="2">
         <v>50</v>
       </c>
       <c r="I80" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>50</v>
       </c>
       <c r="J80" s="2">
@@ -3907,12 +3953,11 @@
         <v>75</v>
       </c>
       <c r="L80" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="13"/>
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>